<commit_message>
first commit on branch
</commit_message>
<xml_diff>
--- a/Excel_Sheets/Maintenance_Duration.xlsx
+++ b/Excel_Sheets/Maintenance_Duration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edima\PycharmProjects\Agenda_Manutencao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrícia\Google Drive (engenharia.ufjf)\5. Pycharm_Projects\Otimizacao_projeto\bat\Excel_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464554E9-F903-4560-9999-8A296E20EE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39A3587-460C-46AD-972A-5F6704623D0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="155">
   <si>
     <t>UG</t>
   </si>
@@ -61,156 +61,6 @@
     <t>OBSERVAÇÃO</t>
   </si>
   <si>
-    <t>UG02</t>
-  </si>
-  <si>
-    <t>UG03</t>
-  </si>
-  <si>
-    <t>UG04</t>
-  </si>
-  <si>
-    <t>UG05</t>
-  </si>
-  <si>
-    <t>UG06</t>
-  </si>
-  <si>
-    <t>UG07</t>
-  </si>
-  <si>
-    <t>UG08</t>
-  </si>
-  <si>
-    <t>UG09</t>
-  </si>
-  <si>
-    <t>UG10</t>
-  </si>
-  <si>
-    <t>UG11</t>
-  </si>
-  <si>
-    <t>UG12</t>
-  </si>
-  <si>
-    <t>UG13</t>
-  </si>
-  <si>
-    <t>UG14</t>
-  </si>
-  <si>
-    <t>UG15</t>
-  </si>
-  <si>
-    <t>UG16</t>
-  </si>
-  <si>
-    <t>UG17</t>
-  </si>
-  <si>
-    <t>UG18</t>
-  </si>
-  <si>
-    <t>UG19</t>
-  </si>
-  <si>
-    <t>UG20</t>
-  </si>
-  <si>
-    <t>UG21</t>
-  </si>
-  <si>
-    <t>UG22</t>
-  </si>
-  <si>
-    <t>UG23</t>
-  </si>
-  <si>
-    <t>UG24</t>
-  </si>
-  <si>
-    <t>UG25</t>
-  </si>
-  <si>
-    <t>UG26</t>
-  </si>
-  <si>
-    <t>UG27</t>
-  </si>
-  <si>
-    <t>UG28</t>
-  </si>
-  <si>
-    <t>UG29</t>
-  </si>
-  <si>
-    <t>UG30</t>
-  </si>
-  <si>
-    <t>UG31</t>
-  </si>
-  <si>
-    <t>UG32</t>
-  </si>
-  <si>
-    <t>UG33</t>
-  </si>
-  <si>
-    <t>UG34</t>
-  </si>
-  <si>
-    <t>UG35</t>
-  </si>
-  <si>
-    <t>UG36</t>
-  </si>
-  <si>
-    <t>UG37</t>
-  </si>
-  <si>
-    <t>UG38</t>
-  </si>
-  <si>
-    <t>UG39</t>
-  </si>
-  <si>
-    <t>UG40</t>
-  </si>
-  <si>
-    <t>UG41</t>
-  </si>
-  <si>
-    <t>UG42</t>
-  </si>
-  <si>
-    <t>UG43</t>
-  </si>
-  <si>
-    <t>UG44</t>
-  </si>
-  <si>
-    <t>UG45</t>
-  </si>
-  <si>
-    <t>UG46</t>
-  </si>
-  <si>
-    <t>UG47</t>
-  </si>
-  <si>
-    <t>UG48</t>
-  </si>
-  <si>
-    <t>UG49</t>
-  </si>
-  <si>
-    <t>UG50</t>
-  </si>
-  <si>
-    <t>UG01</t>
-  </si>
-  <si>
     <t>TRUG</t>
   </si>
   <si>
@@ -232,9 +82,6 @@
     <t>Descrever sucintamente cada atividade a ser realizada.</t>
   </si>
   <si>
-    <t>Preecher com o nome da unidade geradora, lembrando de sempre adicionar o texto "UG" antes de cada número e as unidades de 1 à 9, sempre adicionar o número zero à esquerda (ex.: '04').</t>
-  </si>
-  <si>
     <t>Adicionar observação em relação à atividade realizada.</t>
   </si>
   <si>
@@ -491,6 +338,162 @@
   </si>
   <si>
     <t>PROFISSIONAIS</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG01</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG02</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG03</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG04</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG05</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG06</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG07</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG08</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG09</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG10</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG11</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG12</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG13</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG14</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG15</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG16</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG17</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG18</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG19</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG20</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG21</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG22</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG23</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG24</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG25</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG26</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG27</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG28</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG29</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG30</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG31</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG32</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG33</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG34</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG35</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG36</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG37</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG38</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG39</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG40</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG41</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG42</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG43</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG44</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG45</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG46</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG47</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG48</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG49</t>
+  </si>
+  <si>
+    <t>ROUHSN_13P8_UG50</t>
+  </si>
+  <si>
+    <t>Preecher com o nome da unidade geradora com o seu correto nome, por exemplo "ROUHSN_13P8_UG01".</t>
+  </si>
+  <si>
+    <t>Preencher com o seu respectivo TRUG</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1135,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1153,14 +1156,14 @@
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="18"/>
@@ -1172,17 +1175,17 @@
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>67</v>
+        <v>153</v>
       </c>
       <c r="D6" s="18"/>
     </row>
@@ -1191,9 +1194,11 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="21"/>
+        <v>14</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>154</v>
+      </c>
       <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1203,10 +1208,10 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="20" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D10" s="18"/>
     </row>
@@ -1217,10 +1222,10 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="D12" s="18"/>
     </row>
@@ -1231,10 +1236,10 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="20" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="D14" s="18"/>
     </row>
@@ -1245,10 +1250,10 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="20" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="D16" s="18"/>
     </row>
@@ -1259,10 +1264,10 @@
     </row>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="D18" s="18"/>
     </row>
@@ -1273,35 +1278,35 @@
     </row>
     <row r="20" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="18"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="27" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="D21" s="18"/>
     </row>
     <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="D22" s="18"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="D23" s="18"/>
     </row>
@@ -1343,13 +1348,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H301"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="121.85546875" style="31" bestFit="1" customWidth="1"/>
@@ -1365,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>7</v>
@@ -1377,27 +1382,27 @@
         <v>9</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="F2" s="8">
         <v>53</v>
@@ -1406,16 +1411,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F3" s="8">
         <v>19</v>
@@ -1424,16 +1429,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F4" s="8">
         <v>29</v>
@@ -1442,16 +1447,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="F5" s="8">
         <v>13</v>
@@ -1460,16 +1465,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="F6" s="8">
         <v>18</v>
@@ -1478,16 +1483,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="F7" s="8">
         <v>71</v>
@@ -1496,16 +1501,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="F8" s="8">
         <v>16</v>
@@ -1514,16 +1519,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F9" s="8">
         <v>17</v>
@@ -1532,16 +1537,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F10" s="8">
         <v>6</v>
@@ -1550,31 +1555,31 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="F12" s="8">
         <v>66</v>
@@ -1583,16 +1588,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="F13" s="8">
         <v>32</v>
@@ -1601,16 +1606,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="F14" s="8">
         <v>55</v>
@@ -1619,16 +1624,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F15" s="8">
         <v>36</v>
@@ -1637,16 +1642,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="F16" s="8">
         <v>21</v>
@@ -1655,16 +1660,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="F17" s="8">
         <v>6</v>
@@ -1673,16 +1678,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F18" s="8">
         <v>6</v>
@@ -1691,16 +1696,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="F19" s="8">
         <v>14</v>
@@ -1709,16 +1714,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="F20" s="8">
         <v>17</v>
@@ -1727,16 +1732,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="F21" s="8">
         <v>17</v>
@@ -1745,16 +1750,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F22" s="8">
         <v>6</v>
@@ -1763,16 +1768,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="F23" s="8">
         <v>6</v>
@@ -1781,16 +1786,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="F24" s="8">
         <v>10</v>
@@ -1799,16 +1804,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F25" s="8">
         <v>20</v>
@@ -1817,16 +1822,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="F26" s="8">
         <v>63</v>
@@ -1835,16 +1840,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="F27" s="8">
         <v>23</v>
@@ -1853,16 +1858,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="F28" s="8">
         <v>55</v>
@@ -1871,16 +1876,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="F29" s="8">
         <v>18</v>
@@ -1889,16 +1894,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="F30" s="8">
         <v>18</v>
@@ -1907,16 +1912,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="F31" s="8">
         <v>3</v>
@@ -1925,16 +1930,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="F32" s="8">
         <v>38</v>
@@ -1943,16 +1948,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F33" s="8">
         <v>18</v>
@@ -1961,16 +1966,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="F34" s="8">
         <v>59</v>
@@ -1979,16 +1984,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="F35" s="8">
         <v>30</v>
@@ -1997,16 +2002,16 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F36" s="8">
         <v>14</v>
@@ -2015,16 +2020,16 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="F37" s="4">
         <v>10</v>
@@ -2033,16 +2038,16 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="F38" s="4">
         <v>32</v>
@@ -2051,16 +2056,16 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F39" s="4">
         <v>28</v>
@@ -2069,16 +2074,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="F40" s="4">
         <v>35</v>
@@ -2087,16 +2092,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="F41" s="4">
         <v>3</v>
@@ -2105,16 +2110,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="F42" s="4">
         <v>29</v>
@@ -2123,16 +2128,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="F43" s="4">
         <v>45</v>
@@ -2141,16 +2146,16 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="F44" s="4">
         <v>53</v>
@@ -2159,16 +2164,16 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="F45" s="8">
         <v>4</v>
@@ -2178,16 +2183,16 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="F46" s="8">
         <v>38</v>
@@ -2197,16 +2202,16 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="F47" s="8">
         <v>15</v>
@@ -2216,32 +2221,32 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F49" s="8">
         <v>41</v>
@@ -2250,16 +2255,16 @@
     </row>
     <row r="50" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="E50" s="31"/>
       <c r="F50" s="8">
@@ -2269,16 +2274,16 @@
     </row>
     <row r="51" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="8">
@@ -2288,16 +2293,16 @@
     </row>
     <row r="52" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="8"/>
@@ -2305,16 +2310,16 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="F53" s="8">
         <v>22</v>
@@ -2322,16 +2327,16 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="F54" s="8">
         <v>24</v>
@@ -2339,16 +2344,16 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="F55" s="8">
         <v>25</v>
@@ -2356,16 +2361,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="F56" s="8">
         <v>19</v>
@@ -2373,16 +2378,16 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="F57" s="8">
         <v>6</v>
@@ -2390,16 +2395,16 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="F58" s="8">
         <v>34</v>
@@ -2407,16 +2412,16 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D59" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F59" s="8">
         <v>19</v>
@@ -2424,16 +2429,16 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="F60" s="8">
         <v>5</v>
@@ -2441,16 +2446,16 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F61" s="8">
         <v>24</v>
@@ -2458,16 +2463,16 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F62" s="8">
         <v>22</v>
@@ -2475,16 +2480,16 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="F63" s="8">
         <v>3</v>
@@ -2492,16 +2497,16 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F64" s="8">
         <v>41</v>
@@ -2509,16 +2514,16 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="F65" s="8">
         <v>6</v>
@@ -2526,16 +2531,16 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="F66" s="8">
         <v>29</v>
@@ -2543,16 +2548,16 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F67" s="8">
         <v>6</v>
@@ -2560,16 +2565,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="F68" s="8">
         <v>23</v>
@@ -2577,16 +2582,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="F69" s="8">
         <v>32</v>
@@ -2594,16 +2599,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="F70" s="8">
         <v>6</v>
@@ -2611,16 +2616,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F71" s="8">
         <v>6</v>
@@ -2628,16 +2633,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="F72" s="8">
         <v>74</v>
@@ -2645,16 +2650,16 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="F73" s="8">
         <v>3</v>
@@ -2662,16 +2667,16 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="F74" s="8">
         <v>18</v>
@@ -2679,16 +2684,16 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D75" s="31" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="F75" s="8">
         <v>46</v>
@@ -2696,16 +2701,16 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="31" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="F76" s="8">
         <v>42</v>
@@ -2713,16 +2718,16 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D77" s="31" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="F77" s="8">
         <v>30</v>
@@ -2730,16 +2735,16 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D78" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F78" s="8">
         <v>14</v>
@@ -2747,16 +2752,16 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D79" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F79" s="8">
         <v>29</v>
@@ -2764,16 +2769,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F80" s="8">
         <v>31</v>
@@ -2781,16 +2786,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="F81" s="8">
         <v>27</v>
@@ -2798,16 +2803,16 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D82" s="31" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="F82" s="8">
         <v>27</v>
@@ -2815,16 +2820,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D83" s="31" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="F83" s="8">
         <v>26</v>
@@ -2832,16 +2837,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F84" s="8">
         <v>19</v>
@@ -2849,16 +2854,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D85" s="31" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="F85" s="8">
         <v>24</v>
@@ -2866,16 +2871,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>39</v>
+        <v>133</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D86" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F86" s="8">
         <v>18</v>
@@ -2883,16 +2888,16 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>39</v>
+        <v>133</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D87" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F87" s="8">
         <v>22</v>
@@ -2900,16 +2905,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>39</v>
+        <v>133</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="31" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="F88" s="8">
         <v>27</v>
@@ -2917,16 +2922,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D89" s="31" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="F89" s="8">
         <v>17</v>
@@ -2934,16 +2939,16 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D90" s="31" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="F90" s="8">
         <v>27</v>
@@ -2951,16 +2956,16 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D91" s="31" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="F91" s="8">
         <v>21</v>
@@ -2968,16 +2973,16 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D92" s="31" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="F92" s="8">
         <v>59</v>
@@ -2985,16 +2990,16 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="31" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="F93" s="8">
         <v>30</v>
@@ -3002,16 +3007,16 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D94" s="31" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="F94" s="8">
         <v>6</v>
@@ -3019,16 +3024,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F95" s="8">
         <v>15</v>
@@ -3036,16 +3041,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>41</v>
+        <v>135</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D96" s="31" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="F96" s="8">
         <v>7</v>
@@ -3053,16 +3058,16 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="31" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="F97" s="8">
         <v>3</v>
@@ -3070,16 +3075,16 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D98" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F98" s="8">
         <v>26</v>
@@ -3087,16 +3092,16 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="31" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="F99" s="8">
         <v>7</v>
@@ -3104,16 +3109,16 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="31" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="F100" s="8">
         <v>16</v>
@@ -3121,16 +3126,16 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D101" s="31" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="F101" s="8">
         <v>3</v>
@@ -3138,16 +3143,16 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D102" s="31" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="F102" s="8">
         <v>7</v>
@@ -3155,16 +3160,16 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D103" s="31" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="F103" s="8">
         <v>89</v>
@@ -3172,16 +3177,16 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="31" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="F104" s="8">
         <v>55</v>
@@ -3189,16 +3194,16 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F105" s="8">
         <v>15</v>
@@ -3206,16 +3211,16 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="31" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="F106" s="8">
         <v>29</v>
@@ -3223,16 +3228,16 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D107" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F107" s="8">
         <v>21</v>
@@ -3240,16 +3245,16 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D108" s="31" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="F108" s="8">
         <v>19</v>
@@ -3257,16 +3262,16 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D109" s="31" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="F109" s="8">
         <v>24</v>
@@ -3274,16 +3279,16 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>47</v>
+        <v>141</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D110" s="31" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="F110" s="8">
         <v>18</v>
@@ -3291,16 +3296,16 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>47</v>
+        <v>141</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D111" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F111" s="8">
         <v>18</v>
@@ -3308,16 +3313,16 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>48</v>
+        <v>142</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D112" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F112" s="8">
         <v>22</v>
@@ -3325,16 +3330,16 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F113" s="8">
         <v>6</v>
@@ -3342,16 +3347,16 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D114" s="31" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
       <c r="F114" s="8">
         <v>32</v>
@@ -3359,16 +3364,16 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D115" s="31" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="F115" s="8">
         <v>41</v>
@@ -3376,16 +3381,16 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D116" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F116" s="8">
         <v>24</v>
@@ -3393,16 +3398,16 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D117" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F117" s="8">
         <v>6</v>
@@ -3410,16 +3415,16 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="F118" s="8">
         <v>26</v>
@@ -3427,16 +3432,16 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D119" s="31" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="F119" s="8">
         <v>57</v>
@@ -3444,16 +3449,16 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>51</v>
+        <v>145</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F120" s="8">
         <v>6</v>
@@ -3461,16 +3466,16 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>51</v>
+        <v>145</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D121" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F121" s="8">
         <v>21</v>
@@ -3478,16 +3483,16 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>51</v>
+        <v>145</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="F122" s="8">
         <v>11</v>
@@ -3495,16 +3500,16 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F123" s="8">
         <v>6</v>
@@ -3512,16 +3517,16 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D124" s="31" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="F124" s="8">
         <v>17</v>
@@ -3529,16 +3534,16 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D125" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F125" s="8">
         <v>25</v>
@@ -3546,16 +3551,16 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F126" s="8">
         <v>19</v>
@@ -3563,16 +3568,16 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D127" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F127" s="8">
         <v>19</v>
@@ -3580,16 +3585,16 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D128" s="31" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="F128" s="8">
         <v>40</v>
@@ -3597,16 +3602,16 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D129" s="31" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="F129" s="8">
         <v>3</v>
@@ -3614,16 +3619,16 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D130" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F130" s="8">
         <v>18</v>
@@ -3631,16 +3636,16 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D131" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F131" s="8">
         <v>18</v>
@@ -3648,16 +3653,16 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D132" s="31" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="F132" s="8">
         <v>6</v>
@@ -3665,16 +3670,16 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>55</v>
+        <v>149</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D133" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F133" s="8">
         <v>19</v>
@@ -3682,16 +3687,16 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D134" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F134" s="8">
         <v>8</v>
@@ -3699,16 +3704,16 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D135" s="31" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="F135" s="8">
         <v>88</v>
@@ -3716,16 +3721,16 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D136" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F136" s="8">
         <v>15</v>
@@ -3733,16 +3738,16 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D137" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F137" s="8">
         <v>20</v>
@@ -3750,16 +3755,16 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D138" s="31" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="F138" s="8">
         <v>3</v>
@@ -3767,16 +3772,16 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D139" s="31" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="F139" s="8">
         <v>45</v>
@@ -3784,16 +3789,16 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D140" s="31" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F140" s="8">
         <v>21</v>
@@ -3801,16 +3806,16 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D141" s="31" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="F141" s="8">
         <v>14</v>
@@ -3818,16 +3823,16 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D142" s="31" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="F142" s="8">
         <v>27</v>
@@ -3835,16 +3840,16 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D143" s="31" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="F143" s="8">
         <v>20</v>

</xml_diff>